<commit_message>
Squashed 'seims/src/commonlibs/RasterClass/' changes from 15b7bff00..b759f024f
b759f024f add test of mongodb IO
e54682ae3 Merge branch 'master' of github.com:lreis2415/RasterClass
d5baeb154 update
8c5e88cf5 uupdate
71325679e bugs fixed, e.g. of copy ctor
059dc7252 unittest code

git-subtree-dir: seims/src/commonlibs/RasterClass
git-subtree-split: b759f024fa4d87412bd8e949051e77771039307a
</commit_message>
<xml_diff>
--- a/data/test_dem_values.xlsx
+++ b/data/test_dem_values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10740" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dem_1" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="dem_3" sheetId="4" r:id="rId3"/>
     <sheet name="mask1" sheetId="5" r:id="rId4"/>
     <sheet name="dem_2_mask1" sheetId="6" r:id="rId5"/>
+    <sheet name="dem_1_mask1" sheetId="7" r:id="rId6"/>
+    <sheet name="dem_3_mask1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
   <si>
     <t>min</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -444,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2202,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S8" sqref="J1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3949,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B29"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5693,7 +5695,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6004,7 +6006,7 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B37"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6851,4 +6853,602 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>7.94</v>
+      </c>
+      <c r="B1">
+        <v>7.62</v>
+      </c>
+      <c r="G1">
+        <v>9.43</v>
+      </c>
+      <c r="H1">
+        <v>9.9</v>
+      </c>
+      <c r="I1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J1">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>9.75</v>
+      </c>
+      <c r="B2">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C2">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D2">
+        <v>8.83</v>
+      </c>
+      <c r="E2">
+        <v>8.77</v>
+      </c>
+      <c r="F2">
+        <v>8.31</v>
+      </c>
+      <c r="G2">
+        <v>9.33</v>
+      </c>
+      <c r="H2">
+        <v>7.62</v>
+      </c>
+      <c r="I2">
+        <v>8.43</v>
+      </c>
+      <c r="J2">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>9.64</v>
+      </c>
+      <c r="C3">
+        <v>9.75</v>
+      </c>
+      <c r="D3">
+        <v>7.14</v>
+      </c>
+      <c r="E3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F3">
+        <v>8.89</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>7.14</v>
+      </c>
+      <c r="I3">
+        <v>9.75</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7.07</v>
+      </c>
+      <c r="B4">
+        <v>9.9</v>
+      </c>
+      <c r="C4">
+        <v>9.06</v>
+      </c>
+      <c r="D4">
+        <v>7.21</v>
+      </c>
+      <c r="E4">
+        <v>9.17</v>
+      </c>
+      <c r="F4">
+        <v>7.94</v>
+      </c>
+      <c r="G4">
+        <v>8.6</v>
+      </c>
+      <c r="H4">
+        <v>7.07</v>
+      </c>
+      <c r="I4">
+        <v>8.43</v>
+      </c>
+      <c r="J4">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7.28</v>
+      </c>
+      <c r="B5">
+        <v>8.43</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>9.85</v>
+      </c>
+      <c r="E5">
+        <v>9.59</v>
+      </c>
+      <c r="F5">
+        <v>7.68</v>
+      </c>
+      <c r="G5">
+        <v>8.43</v>
+      </c>
+      <c r="H5">
+        <v>8.19</v>
+      </c>
+      <c r="I5">
+        <v>9.85</v>
+      </c>
+      <c r="J5">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>7.75</v>
+      </c>
+      <c r="C6">
+        <v>9.59</v>
+      </c>
+      <c r="D6">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E6">
+        <v>9.64</v>
+      </c>
+      <c r="I6">
+        <v>9.85</v>
+      </c>
+      <c r="J6">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>7.07</v>
+      </c>
+      <c r="C7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D7">
+        <v>9.85</v>
+      </c>
+      <c r="E7">
+        <v>7.94</v>
+      </c>
+      <c r="I7">
+        <v>8.49</v>
+      </c>
+      <c r="J7">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>7.81</v>
+      </c>
+      <c r="C8">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D8">
+        <v>8.83</v>
+      </c>
+      <c r="E8">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="I8">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="J8">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f>SUMIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>558.9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>COUNTIF(A1:J8,"&gt;-9999")</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>AVERAGEIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>8.7328124999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MIN(A1:J8)</f>
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f>MAX(A1:J8)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(A1:J8)</f>
+        <v>8.7328124999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <f>_xlfn.STDEV.P(A1:J8)</f>
+        <v>0.95102488918205463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B15-B14</f>
+        <v>2.9299999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>7.94</v>
+      </c>
+      <c r="B1">
+        <v>7.62</v>
+      </c>
+      <c r="G1">
+        <v>9.43</v>
+      </c>
+      <c r="H1">
+        <v>9.9</v>
+      </c>
+      <c r="I1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J1">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>9.75</v>
+      </c>
+      <c r="B2">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C2">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D2">
+        <v>8.83</v>
+      </c>
+      <c r="E2">
+        <v>8.77</v>
+      </c>
+      <c r="F2">
+        <v>8.31</v>
+      </c>
+      <c r="G2">
+        <v>9.33</v>
+      </c>
+      <c r="H2">
+        <v>2.62</v>
+      </c>
+      <c r="I2">
+        <v>8.43</v>
+      </c>
+      <c r="J2">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>9.64</v>
+      </c>
+      <c r="C3">
+        <v>9.75</v>
+      </c>
+      <c r="D3">
+        <v>7.14</v>
+      </c>
+      <c r="E3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F3">
+        <v>8.89</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>7.14</v>
+      </c>
+      <c r="I3">
+        <v>9.75</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7.07</v>
+      </c>
+      <c r="B4">
+        <v>9.9</v>
+      </c>
+      <c r="C4">
+        <v>9.06</v>
+      </c>
+      <c r="D4">
+        <v>7.21</v>
+      </c>
+      <c r="E4">
+        <v>9.17</v>
+      </c>
+      <c r="F4">
+        <v>7.94</v>
+      </c>
+      <c r="G4">
+        <v>8.6</v>
+      </c>
+      <c r="H4">
+        <v>7.07</v>
+      </c>
+      <c r="I4">
+        <v>8.43</v>
+      </c>
+      <c r="J4">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>9.59</v>
+      </c>
+      <c r="F5">
+        <v>7.68</v>
+      </c>
+      <c r="G5">
+        <v>8.43</v>
+      </c>
+      <c r="H5">
+        <v>8.19</v>
+      </c>
+      <c r="I5">
+        <v>9.85</v>
+      </c>
+      <c r="J5">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1.75</v>
+      </c>
+      <c r="C6">
+        <v>9.59</v>
+      </c>
+      <c r="D6">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E6">
+        <v>9.64</v>
+      </c>
+      <c r="I6">
+        <v>9.85</v>
+      </c>
+      <c r="J6">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>7.07</v>
+      </c>
+      <c r="C7">
+        <v>1.95</v>
+      </c>
+      <c r="D7">
+        <v>9.85</v>
+      </c>
+      <c r="E7">
+        <v>7.94</v>
+      </c>
+      <c r="I7">
+        <v>8.49</v>
+      </c>
+      <c r="J7">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>7.81</v>
+      </c>
+      <c r="C8">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D8">
+        <v>8.83</v>
+      </c>
+      <c r="E8">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="I8">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="J8">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f>SUMIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>506.34000000000009</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>COUNTIF(A1:J8,"&gt;-9999")</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>AVERAGEIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>8.4390000000000018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MIN(A1:J8)</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f>MAX(A1:J8)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(A1:J8)</f>
+        <v>8.4390000000000018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <f>_xlfn.STDEV.P(A1:J8)</f>
+        <v>1.7183545423844577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B15-B14</f>
+        <v>8.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>